<commit_message>
working on NPOC data
fixing read me for last run, updating processing script
</commit_message>
<xml_diff>
--- a/June_Event/Porewaters/pw_raw_npoc_tn_data/20220819_Readme_COMPASS_SBIR_TEMPEST_AUGMonthly_n32_Leiden_n6.xlsx
+++ b/June_Event/Porewaters/pw_raw_npoc_tn_data/20220819_Readme_COMPASS_SBIR_TEMPEST_AUGMonthly_n32_Leiden_n6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl.sharepoint.com/teams/MCRL-COMPASS/Shared Documents/2.3 TEMPEST/NPOCTN_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myer056/OneDrive - PNNL/Documents/GitHub/TEMPEST/June_Event/Porewaters/pw_raw_npoc_tn_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E73F8F9D-9C01-264C-891F-3FDDA44BBF76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015E1E13-D148-0C45-B363-38D29B792D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{504CB6CD-F08C-074A-B262-93F6352CE28F}"/>
+    <workbookView xWindow="30980" yWindow="1880" windowWidth="31120" windowHeight="14580" xr2:uid="{504CB6CD-F08C-074A-B262-93F6352CE28F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="79">
   <si>
     <t>Sample Name</t>
   </si>
@@ -70,120 +70,24 @@
     <t>CKSTD1_1ppmCN</t>
   </si>
   <si>
-    <t>C_H3_20220808</t>
-  </si>
-  <si>
-    <t>C_H6_20220808</t>
-  </si>
-  <si>
-    <t>C_B4_20220808</t>
-  </si>
-  <si>
-    <t>C_D5_20220808</t>
-  </si>
-  <si>
-    <t>C_E3_20220808</t>
-  </si>
-  <si>
-    <t>C_F6_20220808</t>
-  </si>
-  <si>
-    <t>C_I5_20220808</t>
-  </si>
-  <si>
-    <t>C_C3_20220808</t>
-  </si>
-  <si>
-    <t>C_C6_20220808</t>
-  </si>
-  <si>
-    <t>C_F4_20220808</t>
-  </si>
-  <si>
     <t>Blank2</t>
   </si>
   <si>
     <t>CKSTD2_1ppmCN</t>
   </si>
   <si>
-    <t>FW_C3_20220808</t>
-  </si>
-  <si>
-    <t>FW_C6_20220808</t>
-  </si>
-  <si>
-    <t>FW_F4_20220808</t>
-  </si>
-  <si>
-    <t>FW_H3_20220808</t>
-  </si>
-  <si>
-    <t>FW_H6_20220808</t>
-  </si>
-  <si>
-    <t>FW_B4_20220808</t>
-  </si>
-  <si>
-    <t>FW_D5_20220808</t>
-  </si>
-  <si>
-    <t>FW_E3_20220808</t>
-  </si>
-  <si>
-    <t>SW_H3_20220811_EXTRA</t>
-  </si>
-  <si>
-    <t>FW_I5_20220808</t>
-  </si>
-  <si>
     <t>Blank3</t>
   </si>
   <si>
     <t>CKSTD3_1ppmCN</t>
   </si>
   <si>
-    <t>C_POOLED_20220808</t>
-  </si>
-  <si>
-    <t>SW_F4_20220808</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SW_H3_20220811 </t>
-  </si>
-  <si>
-    <t>SW_H6_20220808</t>
-  </si>
-  <si>
-    <t>SW_B4_20220808</t>
-  </si>
-  <si>
-    <t>SW_D5_20220808</t>
-  </si>
-  <si>
-    <t>SW_F6_20220808</t>
-  </si>
-  <si>
-    <t>SW_I5_20220808</t>
-  </si>
-  <si>
-    <t>SW_C3_20220808</t>
-  </si>
-  <si>
-    <t>SW_POOLED_20220808</t>
-  </si>
-  <si>
     <t>Blank4</t>
   </si>
   <si>
     <t>CKSTD4_1ppmCN</t>
   </si>
   <si>
-    <t>FW_POOLED_20220808</t>
-  </si>
-  <si>
-    <t>SW_E3_20220808</t>
-  </si>
-  <si>
     <t>Leiden_BC11_MCRLRep9</t>
   </si>
   <si>
@@ -266,6 +170,108 @@
   </si>
   <si>
     <t>NPOC: 2.043 mg/L, TN: 0.9605 mg/L</t>
+  </si>
+  <si>
+    <t>Sample wt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total vol: </t>
+  </si>
+  <si>
+    <t>TMP_C_H3_20220808</t>
+  </si>
+  <si>
+    <t>TMP_C_H6_20220808</t>
+  </si>
+  <si>
+    <t>TMP_C_B4_20220808</t>
+  </si>
+  <si>
+    <t>TMP_C_D5_20220808</t>
+  </si>
+  <si>
+    <t>TMP_C_E3_20220808</t>
+  </si>
+  <si>
+    <t>TMP_C_F6_20220808</t>
+  </si>
+  <si>
+    <t>TMP_C_I5_20220808</t>
+  </si>
+  <si>
+    <t>TMP_C_C3_20220808</t>
+  </si>
+  <si>
+    <t>TMP_C_C6_20220808</t>
+  </si>
+  <si>
+    <t>TMP_C_F4_20220808</t>
+  </si>
+  <si>
+    <t>TMP_FW_C3_20220808</t>
+  </si>
+  <si>
+    <t>TMP_FW_C6_20220808</t>
+  </si>
+  <si>
+    <t>TMP_FW_F4_20220808</t>
+  </si>
+  <si>
+    <t>TMP_FW_H3_20220808</t>
+  </si>
+  <si>
+    <t>TMP_FW_H6_20220808</t>
+  </si>
+  <si>
+    <t>TMP_FW_B4_20220808</t>
+  </si>
+  <si>
+    <t>TMP_FW_D5_20220808</t>
+  </si>
+  <si>
+    <t>TMP_FW_E3_20220808</t>
+  </si>
+  <si>
+    <t>TMP_SW_H3_20220811_EXTRA</t>
+  </si>
+  <si>
+    <t>TMP_FW_I5_20220808</t>
+  </si>
+  <si>
+    <t>TMP_C_POOLED_20220808</t>
+  </si>
+  <si>
+    <t>TMP_SW_F4_20220808</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMP_SW_H3_20220811 </t>
+  </si>
+  <si>
+    <t>TMP_SW_H6_20220808</t>
+  </si>
+  <si>
+    <t>TMP_SW_B4_20220808</t>
+  </si>
+  <si>
+    <t>TMP_SW_D5_20220808</t>
+  </si>
+  <si>
+    <t>TMP_SW_F6_20220808</t>
+  </si>
+  <si>
+    <t>TMP_SW_I5_20220808</t>
+  </si>
+  <si>
+    <t>TMP_SW_C3_20220808</t>
+  </si>
+  <si>
+    <t>TMP_SW_POOLED_20220808</t>
+  </si>
+  <si>
+    <t>TMP_FW_POOLED_20220808</t>
+  </si>
+  <si>
+    <t>TMP_SW_E3_20220808</t>
   </si>
 </sst>
 </file>
@@ -617,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B19A6F76-BDE5-5C41-8014-93B9A742975C}">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -630,7 +636,7 @@
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -643,8 +649,14 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -652,10 +664,10 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -663,7 +675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -671,29 +683,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -701,13 +713,13 @@
         <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -715,548 +727,548 @@
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="B9">
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B10">
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="B11">
         <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="B12">
         <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="B13">
         <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="B14">
         <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="B15">
         <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="B16">
         <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="B17">
         <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="B18">
         <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B19">
         <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B20">
         <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="B21">
         <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="B22">
         <v>42</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="B23">
         <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="B24">
         <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="B25">
         <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="B26">
         <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="B27">
         <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="D27" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="B28">
         <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="B29">
         <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="B30">
         <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="B31">
         <v>51</v>
       </c>
       <c r="C31" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="B32">
         <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="B33">
         <v>53</v>
       </c>
       <c r="C33" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="B34">
         <v>54</v>
       </c>
       <c r="C34" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="B35">
         <v>55</v>
       </c>
       <c r="C35" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="B36">
         <v>56</v>
       </c>
       <c r="C36" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="B37">
         <v>57</v>
       </c>
       <c r="C37" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="B38">
         <v>58</v>
       </c>
       <c r="C38" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="B39">
         <v>59</v>
       </c>
       <c r="C39" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="B40">
         <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="B41">
         <v>61</v>
       </c>
       <c r="C41" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="B42">
         <v>62</v>
       </c>
       <c r="C42" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="B43">
         <v>63</v>
       </c>
       <c r="C43" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="D43" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="B44">
         <v>64</v>
       </c>
       <c r="C44" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="D44" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="B45">
         <v>65</v>
       </c>
       <c r="C45" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="B46">
         <v>66</v>
       </c>
       <c r="C46" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="B47">
         <v>67</v>
       </c>
       <c r="C47" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="B48">
         <v>68</v>
       </c>
       <c r="C48" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="B49">
         <v>69</v>
       </c>
       <c r="C49" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="B50">
         <v>70</v>
       </c>
       <c r="C50" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="B51">
         <v>71</v>
       </c>
       <c r="C51" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="B52">
         <v>72</v>
       </c>
       <c r="C52" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="B53">
         <v>73</v>
       </c>
       <c r="C53" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="D53" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="B54">
         <v>74</v>
       </c>
       <c r="C54" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="D54" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -1264,7 +1276,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -1272,7 +1284,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="B57">
         <v>0</v>

</xml_diff>